<commit_message>
inserting a blank row so Nick doesnt have a fit
</commit_message>
<xml_diff>
--- a/doc/template_0_2_0.xlsx
+++ b/doc/template_0_2_0.xlsx
@@ -3547,7 +3547,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3601,18 +3601,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3623,6 +3611,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5356,16 +5359,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="34" customWidth="1"/>
     <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
@@ -5374,7 +5377,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
-      <c r="B1" s="27"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="23" t="s">
@@ -5385,7 +5388,7 @@
       <c r="A2" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -5394,7 +5397,7 @@
       <c r="A3" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="34" t="s">
         <v>637</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -5405,7 +5408,7 @@
       <c r="A4" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="33" t="s">
         <v>555</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -5416,7 +5419,7 @@
       <c r="A5" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="33" t="s">
         <v>638</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -5427,7 +5430,7 @@
       <c r="A6" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="33" t="s">
         <v>649</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -5438,7 +5441,7 @@
       <c r="A7" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="33" t="s">
         <v>448</v>
       </c>
       <c r="C7" s="3" t="str">
@@ -5457,7 +5460,7 @@
       <c r="A8" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="33" t="s">
         <v>449</v>
       </c>
       <c r="C8" s="3" t="str">
@@ -5476,7 +5479,7 @@
       <c r="A9" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="33">
         <v>2</v>
       </c>
       <c r="C9" s="3"/>
@@ -5489,7 +5492,7 @@
       <c r="A11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="12"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -5498,7 +5501,7 @@
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="33" t="s">
         <v>648</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -5509,7 +5512,7 @@
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="33" t="s">
         <v>471</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -5520,7 +5523,7 @@
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="33" t="s">
         <v>472</v>
       </c>
     </row>
@@ -5528,7 +5531,7 @@
       <c r="A15" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B15" s="25" t="b">
+      <c r="B15" s="33" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -5539,7 +5542,7 @@
       <c r="A16" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B16" s="28" t="b">
+      <c r="B16" s="32" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -5550,7 +5553,7 @@
       <c r="A17" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="33" t="s">
         <v>492</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -5561,7 +5564,7 @@
       <c r="A18" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="33" t="s">
         <v>604</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -5569,13 +5572,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="25"/>
+      <c r="B19" s="33"/>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="14" t="s">
@@ -5586,15 +5589,15 @@
       <c r="A21" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>602</v>
+      <c r="B21" s="33" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="14" t="s">
@@ -5605,7 +5608,7 @@
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="33" t="s">
         <v>476</v>
       </c>
     </row>
@@ -5613,181 +5616,181 @@
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="33">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="38" t="str">
+      <c r="A26" s="39" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,1,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,1,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+        <v>popSize</v>
+      </c>
+      <c r="B26" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,1,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,1,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+        <v>Generations</v>
+      </c>
+      <c r="B27" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+        <v>5</v>
+      </c>
+      <c r="C27" s="39"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+        <v>waitGenerations</v>
+      </c>
+      <c r="B28" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+        <v>solutionTolerance</v>
+      </c>
+      <c r="B29" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
         <v>epsilonGradient</v>
       </c>
-      <c r="B26" s="38">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,1,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,1,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+      <c r="B30" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+    <row r="31" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
         <v>pgtol</v>
       </c>
-      <c r="B27" s="38">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,2,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+      <c r="B31" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
         <v>0.01</v>
       </c>
-      <c r="C27" s="38">
-        <f>MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+    </row>
+    <row r="32" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
         <v>factr</v>
       </c>
-      <c r="B28" s="38">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,3,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+      <c r="B32" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
         <v>45036000000000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+    <row r="33" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
         <v>maxit</v>
       </c>
-      <c r="B29" s="38">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,4,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+      <c r="B33" s="34">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+    <row r="34" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
         <v>normType</v>
       </c>
-      <c r="B30" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,5,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
+      <c r="B34" s="34" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
         <v>minkowski</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="39" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,10,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,10,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
         <v>pPower</v>
       </c>
-      <c r="B31" s="38">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,6,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
-        <v/>
-      </c>
-      <c r="B32" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,7,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
-        <v/>
-      </c>
-      <c r="B33" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,8,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
-        <v/>
-      </c>
-      <c r="B34" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,9,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,10,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))=0,"",INDEX(Lookups!$C$12:$L$21,10,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)-1))</f>
-        <v/>
-      </c>
-      <c r="B35" s="38" t="str">
+      <c r="B35" s="34">
         <f>IF(LEN(INDEX(Lookups!$C$12:$L$21,10,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))=0,"",INDEX(Lookups!$C$12:$L$21,10,2*MATCH(Setup!$B21,Lookups!$A$12:$A$18,0)))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="34"/>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B37" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="14"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="D37" s="12"/>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B38" s="33" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+    <row r="40" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B40" s="35" t="s">
         <v>475</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D40" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E40" s="14" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="34" t="s">
         <v>632</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D41" s="24" t="s">
         <v>631</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
+    <row r="43" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B43" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="14"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -5872,28 +5875,28 @@
       <c r="H1" s="6"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="25" t="s">
         <v>503</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="31" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="27" t="s">
         <v>504</v>
       </c>
-      <c r="Q1" s="32"/>
+      <c r="Q1" s="28"/>
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -7497,17 +7500,17 @@
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="33"/>
+      <c r="K57" s="29"/>
+      <c r="L57" s="29"/>
+      <c r="M57" s="29"/>
+      <c r="N57" s="29"/>
+      <c r="O57" s="29"/>
       <c r="P57" s="1"/>
-      <c r="Q57" s="33"/>
-      <c r="R57" s="33"/>
-      <c r="S57" s="33"/>
-      <c r="T57" s="33"/>
-      <c r="U57" s="33"/>
+      <c r="Q57" s="29"/>
+      <c r="R57" s="29"/>
+      <c r="S57" s="29"/>
+      <c r="T57" s="29"/>
+      <c r="U57" s="29"/>
     </row>
     <row r="58" spans="1:21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="20"/>
@@ -7535,16 +7538,16 @@
         <v>439</v>
       </c>
       <c r="K58" s="20"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33"/>
-      <c r="O58" s="33"/>
+      <c r="L58" s="29"/>
+      <c r="M58" s="29"/>
+      <c r="N58" s="29"/>
+      <c r="O58" s="29"/>
       <c r="P58" s="1"/>
-      <c r="Q58" s="33"/>
-      <c r="R58" s="33"/>
-      <c r="S58" s="33"/>
-      <c r="T58" s="33"/>
-      <c r="U58" s="33"/>
+      <c r="Q58" s="29"/>
+      <c r="R58" s="29"/>
+      <c r="S58" s="29"/>
+      <c r="T58" s="29"/>
+      <c r="U58" s="29"/>
     </row>
     <row r="59" spans="1:21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="20"/>
@@ -7569,13 +7572,13 @@
         <v>1</v>
       </c>
       <c r="J59" s="20"/>
-      <c r="K59" s="34">
+      <c r="K59" s="30">
         <v>-2</v>
       </c>
-      <c r="L59" s="34">
-        <v>2</v>
-      </c>
-      <c r="M59" s="34">
+      <c r="L59" s="30">
+        <v>2</v>
+      </c>
+      <c r="M59" s="30">
         <v>0</v>
       </c>
       <c r="N59" s="3">
@@ -7584,13 +7587,13 @@
       </c>
       <c r="O59" s="3"/>
       <c r="P59" s="1"/>
-      <c r="Q59" s="33"/>
-      <c r="R59" s="33" t="s">
+      <c r="Q59" s="29"/>
+      <c r="R59" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="S59" s="33"/>
-      <c r="T59" s="33"/>
-      <c r="U59" s="33"/>
+      <c r="S59" s="29"/>
+      <c r="T59" s="29"/>
+      <c r="U59" s="29"/>
     </row>
     <row r="60" spans="1:21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" t="b">
@@ -7611,17 +7614,17 @@
       <c r="H60" s="20"/>
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="33"/>
-      <c r="O60" s="33"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="29"/>
+      <c r="O60" s="29"/>
       <c r="P60" s="1"/>
-      <c r="Q60" s="33"/>
-      <c r="R60" s="33"/>
-      <c r="S60" s="33"/>
-      <c r="T60" s="33"/>
-      <c r="U60" s="33"/>
+      <c r="Q60" s="29"/>
+      <c r="R60" s="29"/>
+      <c r="S60" s="29"/>
+      <c r="T60" s="29"/>
+      <c r="U60" s="29"/>
     </row>
     <row r="61" spans="1:21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="20"/>
@@ -7649,16 +7652,16 @@
         <v>439</v>
       </c>
       <c r="K61" s="20"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="33"/>
-      <c r="N61" s="33"/>
-      <c r="O61" s="33"/>
+      <c r="L61" s="29"/>
+      <c r="M61" s="29"/>
+      <c r="N61" s="29"/>
+      <c r="O61" s="29"/>
       <c r="P61" s="1"/>
-      <c r="Q61" s="33"/>
-      <c r="R61" s="33"/>
-      <c r="S61" s="33"/>
-      <c r="T61" s="33"/>
-      <c r="U61" s="33"/>
+      <c r="Q61" s="29"/>
+      <c r="R61" s="29"/>
+      <c r="S61" s="29"/>
+      <c r="T61" s="29"/>
+      <c r="U61" s="29"/>
     </row>
     <row r="62" spans="1:21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="20"/>
@@ -7683,13 +7686,13 @@
         <v>1</v>
       </c>
       <c r="J62" s="20"/>
-      <c r="K62" s="34">
+      <c r="K62" s="30">
         <v>-2</v>
       </c>
-      <c r="L62" s="34">
-        <v>2</v>
-      </c>
-      <c r="M62" s="34">
+      <c r="L62" s="30">
+        <v>2</v>
+      </c>
+      <c r="M62" s="30">
         <v>0</v>
       </c>
       <c r="N62" s="3">
@@ -7698,13 +7701,13 @@
       </c>
       <c r="O62" s="3"/>
       <c r="P62" s="1"/>
-      <c r="Q62" s="33"/>
-      <c r="R62" s="33" t="s">
+      <c r="Q62" s="29"/>
+      <c r="R62" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="S62" s="33"/>
-      <c r="T62" s="33"/>
-      <c r="U62" s="33"/>
+      <c r="S62" s="29"/>
+      <c r="T62" s="29"/>
+      <c r="U62" s="29"/>
     </row>
     <row r="63" spans="1:21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" t="b">
@@ -7725,17 +7728,17 @@
       <c r="H63" s="20"/>
       <c r="I63" s="20"/>
       <c r="J63" s="20"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
-      <c r="O63" s="33"/>
+      <c r="K63" s="29"/>
+      <c r="L63" s="29"/>
+      <c r="M63" s="29"/>
+      <c r="N63" s="29"/>
+      <c r="O63" s="29"/>
       <c r="P63" s="1"/>
-      <c r="Q63" s="33"/>
-      <c r="R63" s="33"/>
-      <c r="S63" s="33"/>
-      <c r="T63" s="33"/>
-      <c r="U63" s="33"/>
+      <c r="Q63" s="29"/>
+      <c r="R63" s="29"/>
+      <c r="S63" s="29"/>
+      <c r="T63" s="29"/>
+      <c r="U63" s="29"/>
     </row>
     <row r="64" spans="1:21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
@@ -7763,16 +7766,16 @@
         <v>439</v>
       </c>
       <c r="K64" s="20"/>
-      <c r="L64" s="33"/>
-      <c r="M64" s="33"/>
-      <c r="N64" s="33"/>
-      <c r="O64" s="33"/>
+      <c r="L64" s="29"/>
+      <c r="M64" s="29"/>
+      <c r="N64" s="29"/>
+      <c r="O64" s="29"/>
       <c r="P64" s="1"/>
-      <c r="Q64" s="33"/>
-      <c r="R64" s="33"/>
-      <c r="S64" s="33"/>
-      <c r="T64" s="33"/>
-      <c r="U64" s="33"/>
+      <c r="Q64" s="29"/>
+      <c r="R64" s="29"/>
+      <c r="S64" s="29"/>
+      <c r="T64" s="29"/>
+      <c r="U64" s="29"/>
     </row>
     <row r="65" spans="1:24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
@@ -7797,13 +7800,13 @@
         <v>1</v>
       </c>
       <c r="J65" s="20"/>
-      <c r="K65" s="34">
+      <c r="K65" s="30">
         <v>-2</v>
       </c>
-      <c r="L65" s="34">
-        <v>2</v>
-      </c>
-      <c r="M65" s="34">
+      <c r="L65" s="30">
+        <v>2</v>
+      </c>
+      <c r="M65" s="30">
         <v>0</v>
       </c>
       <c r="N65" s="3">
@@ -7812,13 +7815,13 @@
       </c>
       <c r="O65" s="3"/>
       <c r="P65" s="1"/>
-      <c r="Q65" s="33"/>
-      <c r="R65" s="33" t="s">
+      <c r="Q65" s="29"/>
+      <c r="R65" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="S65" s="33"/>
-      <c r="T65" s="33"/>
-      <c r="U65" s="33"/>
+      <c r="S65" s="29"/>
+      <c r="T65" s="29"/>
+      <c r="U65" s="29"/>
     </row>
     <row r="66" spans="1:24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" t="b">
@@ -7839,17 +7842,17 @@
       <c r="H66" s="20"/>
       <c r="I66" s="20"/>
       <c r="J66" s="20"/>
-      <c r="K66" s="33"/>
-      <c r="L66" s="33"/>
-      <c r="M66" s="33"/>
-      <c r="N66" s="33"/>
-      <c r="O66" s="33"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="29"/>
+      <c r="M66" s="29"/>
+      <c r="N66" s="29"/>
+      <c r="O66" s="29"/>
       <c r="P66" s="1"/>
-      <c r="Q66" s="33"/>
-      <c r="R66" s="33"/>
-      <c r="S66" s="33"/>
-      <c r="T66" s="33"/>
-      <c r="U66" s="33"/>
+      <c r="Q66" s="29"/>
+      <c r="R66" s="29"/>
+      <c r="S66" s="29"/>
+      <c r="T66" s="29"/>
+      <c r="U66" s="29"/>
     </row>
     <row r="67" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="20"/>
@@ -7877,18 +7880,18 @@
         <v>439</v>
       </c>
       <c r="K67" s="20"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="33"/>
-      <c r="N67" s="33"/>
-      <c r="O67" s="33"/>
-      <c r="Q67" s="33"/>
-      <c r="R67" s="33"/>
-      <c r="S67" s="33"/>
-      <c r="T67" s="33"/>
-      <c r="U67" s="33"/>
-      <c r="V67" s="33"/>
-      <c r="W67" s="33"/>
-      <c r="X67" s="33"/>
+      <c r="L67" s="29"/>
+      <c r="M67" s="29"/>
+      <c r="N67" s="29"/>
+      <c r="O67" s="29"/>
+      <c r="Q67" s="29"/>
+      <c r="R67" s="29"/>
+      <c r="S67" s="29"/>
+      <c r="T67" s="29"/>
+      <c r="U67" s="29"/>
+      <c r="V67" s="29"/>
+      <c r="W67" s="29"/>
+      <c r="X67" s="29"/>
     </row>
     <row r="68" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="20"/>
@@ -7913,13 +7916,13 @@
         <v>1</v>
       </c>
       <c r="J68" s="20"/>
-      <c r="K68" s="34">
+      <c r="K68" s="30">
         <v>-2</v>
       </c>
-      <c r="L68" s="34">
-        <v>2</v>
-      </c>
-      <c r="M68" s="34">
+      <c r="L68" s="30">
+        <v>2</v>
+      </c>
+      <c r="M68" s="30">
         <v>0</v>
       </c>
       <c r="N68" s="3">
@@ -7927,16 +7930,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="O68" s="3"/>
-      <c r="Q68" s="33"/>
-      <c r="R68" s="33" t="s">
+      <c r="Q68" s="29"/>
+      <c r="R68" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="S68" s="33"/>
-      <c r="T68" s="33"/>
-      <c r="U68" s="33"/>
-      <c r="V68" s="33"/>
-      <c r="W68" s="33"/>
-      <c r="X68" s="33"/>
+      <c r="S68" s="29"/>
+      <c r="T68" s="29"/>
+      <c r="U68" s="29"/>
+      <c r="V68" s="29"/>
+      <c r="W68" s="29"/>
+      <c r="X68" s="29"/>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69" t="b">
@@ -7959,9 +7962,9 @@
       <c r="J69"/>
       <c r="K69"/>
       <c r="L69"/>
-      <c r="V69" s="33"/>
-      <c r="W69" s="33"/>
-      <c r="X69" s="33"/>
+      <c r="V69" s="29"/>
+      <c r="W69" s="29"/>
+      <c r="X69" s="29"/>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70"/>
@@ -7990,9 +7993,9 @@
       </c>
       <c r="K70"/>
       <c r="L70"/>
-      <c r="V70" s="33"/>
-      <c r="W70" s="33"/>
-      <c r="X70" s="33"/>
+      <c r="V70" s="29"/>
+      <c r="W70" s="29"/>
+      <c r="X70" s="29"/>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71"/>
@@ -8019,9 +8022,9 @@
       <c r="J71"/>
       <c r="K71"/>
       <c r="L71"/>
-      <c r="V71" s="33"/>
-      <c r="W71" s="33"/>
-      <c r="X71" s="33"/>
+      <c r="V71" s="29"/>
+      <c r="W71" s="29"/>
+      <c r="X71" s="29"/>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72"/>
@@ -8060,13 +8063,13 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="O72" s="3"/>
-      <c r="Q72" s="33"/>
-      <c r="R72" s="33" t="s">
+      <c r="Q72" s="29"/>
+      <c r="R72" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="V72" s="33"/>
-      <c r="W72" s="33"/>
-      <c r="X72" s="33"/>
+      <c r="V72" s="29"/>
+      <c r="W72" s="29"/>
+      <c r="X72" s="29"/>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73"/>
@@ -8093,9 +8096,9 @@
       <c r="J73"/>
       <c r="K73"/>
       <c r="L73"/>
-      <c r="V73" s="33"/>
-      <c r="W73" s="33"/>
-      <c r="X73" s="33"/>
+      <c r="V73" s="29"/>
+      <c r="W73" s="29"/>
+      <c r="X73" s="29"/>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74"/>
@@ -8122,9 +8125,9 @@
       <c r="J74"/>
       <c r="K74"/>
       <c r="L74"/>
-      <c r="V74" s="33"/>
-      <c r="W74" s="33"/>
-      <c r="X74" s="33"/>
+      <c r="V74" s="29"/>
+      <c r="W74" s="29"/>
+      <c r="X74" s="29"/>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75"/>
@@ -8153,9 +8156,9 @@
       </c>
       <c r="K75"/>
       <c r="L75"/>
-      <c r="V75" s="33"/>
-      <c r="W75" s="33"/>
-      <c r="X75" s="33"/>
+      <c r="V75" s="29"/>
+      <c r="W75" s="29"/>
+      <c r="X75" s="29"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76"/>
@@ -8184,9 +8187,9 @@
       </c>
       <c r="K76"/>
       <c r="L76"/>
-      <c r="V76" s="33"/>
-      <c r="W76" s="33"/>
-      <c r="X76" s="33"/>
+      <c r="V76" s="29"/>
+      <c r="W76" s="29"/>
+      <c r="X76" s="29"/>
     </row>
     <row r="77" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" t="b">
@@ -8726,9 +8729,9 @@
       <c r="S95"/>
       <c r="T95"/>
       <c r="U95"/>
-      <c r="V95" s="33"/>
-      <c r="W95" s="33"/>
-      <c r="X95" s="33"/>
+      <c r="V95" s="29"/>
+      <c r="W95" s="29"/>
+      <c r="X95" s="29"/>
     </row>
     <row r="96" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
@@ -8766,8 +8769,8 @@
         <v>5</v>
       </c>
       <c r="P96" s="1"/>
-      <c r="Q96" s="33"/>
-      <c r="R96" s="33" t="s">
+      <c r="Q96" s="29"/>
+      <c r="R96" s="29" t="s">
         <v>27</v>
       </c>
     </row>
@@ -17735,7 +17738,7 @@
       <c r="G12" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="37">
         <v>0.01</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -17744,7 +17747,7 @@
       <c r="J12">
         <v>30</v>
       </c>
-      <c r="K12" s="38" t="s">
+      <c r="K12" s="39" t="s">
         <v>658</v>
       </c>
       <c r="L12">
@@ -17758,16 +17761,16 @@
       <c r="G13" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="37">
         <v>0.01</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="39" t="s">
         <v>658</v>
       </c>
       <c r="J13">
         <v>5</v>
       </c>
-      <c r="K13" s="38" t="s">
+      <c r="K13" s="39" t="s">
         <v>659</v>
       </c>
       <c r="L13">
@@ -17781,7 +17784,7 @@
       <c r="G14" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="37">
         <v>45036000000000</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -17790,7 +17793,7 @@
       <c r="J14">
         <v>3</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="39" t="s">
         <v>660</v>
       </c>
       <c r="L14">
@@ -17810,10 +17813,10 @@
       <c r="I15" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="J15" s="36">
+      <c r="J15" s="37">
         <v>0.01</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="39" t="s">
         <v>661</v>
       </c>
       <c r="L15">
@@ -17827,16 +17830,16 @@
       <c r="G16" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="39" t="s">
         <v>600</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="J16" s="36">
+      <c r="J16" s="37">
         <v>0.01</v>
       </c>
-      <c r="K16" s="38" t="s">
+      <c r="K16" s="39" t="s">
         <v>662</v>
       </c>
       <c r="L16">
@@ -17850,19 +17853,19 @@
       <c r="G17" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="39">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="J17" s="36">
+      <c r="J17" s="37">
         <v>0.01</v>
       </c>
-      <c r="K17" s="38" t="s">
+      <c r="K17" s="39" t="s">
         <v>599</v>
       </c>
-      <c r="L17" s="38" t="s">
+      <c r="L17" s="39" t="s">
         <v>600</v>
       </c>
     </row>
@@ -17873,13 +17876,13 @@
       <c r="I18" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="J18" s="36">
+      <c r="J18" s="37">
         <v>45036000000000</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="K18" s="39" t="s">
         <v>601</v>
       </c>
-      <c r="L18" s="38">
+      <c r="L18" s="39">
         <v>2</v>
       </c>
     </row>
@@ -17887,7 +17890,7 @@
       <c r="I19" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="J19" s="37">
+      <c r="J19" s="38">
         <v>100</v>
       </c>
     </row>
@@ -17895,7 +17898,7 @@
       <c r="I20" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="J20" s="38" t="s">
+      <c r="J20" s="39" t="s">
         <v>600</v>
       </c>
     </row>
@@ -17903,7 +17906,7 @@
       <c r="I21" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="J21" s="38">
+      <c r="J21" s="39">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated 2.0 template_0_2_0.xlsx for dropdown menus
</commit_message>
<xml_diff>
--- a/doc/template_0_2_0.xlsx
+++ b/doc/template_0_2_0.xlsx
@@ -18,10 +18,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$G$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$AA$15</definedName>
     <definedName name="AnalysisType">Lookups!$A$13:$A$19</definedName>
-    <definedName name="nsga">Lookups!$K$14:$L$20</definedName>
-    <definedName name="nsga_nrel">Lookups!$K$14:$L$20</definedName>
-    <definedName name="optim">Lookups!$G$13:$H$18</definedName>
-    <definedName name="rgenoud">Lookups!$I$13:$J$22</definedName>
+    <definedName name="nsga">Lookups!$O$14:$P$20</definedName>
+    <definedName name="nsga_nrel">Lookups!$O$14:$P$20</definedName>
+    <definedName name="optim">Lookups!$I$13:$J$18</definedName>
+    <definedName name="rgenoud">Lookups!$L$13:$M$22</definedName>
     <definedName name="samplemethod">Lookups!$A$8:$A$10</definedName>
     <definedName name="SensitivityType">Lookups!$A$8:$A$9</definedName>
     <definedName name="sentivity">Lookups!$A$8:$A$9</definedName>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2506" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="663">
   <si>
     <t>type</t>
   </si>
@@ -2019,6 +2019,9 @@
   </si>
   <si>
     <t>SensitivityType</t>
+  </si>
+  <si>
+    <t>Sample Method</t>
   </si>
 </sst>
 </file>
@@ -5361,7 +5364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -5594,10 +5597,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="str">
-        <f>IF(IF(ISNA(MATCH($B$21,Lookups!A14,0)),0,1),"Sample Method","")</f>
-        <v>Sample Method</v>
-      </c>
+      <c r="A22" s="38"/>
     </row>
     <row r="23" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="33"/>
@@ -5615,107 +5615,146 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,1,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,1,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
-        <v>Number of Samples</v>
-      </c>
-      <c r="B25" s="33">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,1,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,1,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
-        <v>30</v>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
+        <v>Sample Method</v>
+      </c>
+      <c r="B25" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v>individual_variables</v>
+      </c>
+      <c r="C25" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,2,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,2,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
+        <v>Number of Samples</v>
+      </c>
+      <c r="B26" s="38">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v>30</v>
+      </c>
+      <c r="C26" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
-      <c r="B26" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,2,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,2,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
-        <v/>
-      </c>
-      <c r="C26" s="38"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,3,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,3,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B27" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,3,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,3,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B27" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v/>
+      </c>
+      <c r="C27" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,4,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,4,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B28" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,4,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,4,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B28" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v/>
+      </c>
+      <c r="C28" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,5,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,5,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B29" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,5,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,5,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B29" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v/>
+      </c>
+      <c r="C29" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,6,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,6,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B30" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,6,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,6,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B30" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v/>
+      </c>
+      <c r="C30" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,7,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,7,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B31" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,7,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,7,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B31" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v/>
+      </c>
+      <c r="C31" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,8,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,8,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B32" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,8,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,8,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B32" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v/>
+      </c>
+      <c r="C32" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,9,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,9,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B33" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,9,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,9,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B33" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <v/>
+      </c>
+      <c r="C33" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="38" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,10,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$L$22,10,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))=0,"",INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-2))</f>
         <v/>
       </c>
-      <c r="B34" s="33" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$L$22,10,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$L$22,10,2*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+      <c r="B34" s="38" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
         <v/>
       </c>
+      <c r="C34" s="33" t="str">
+        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -5786,7 +5825,7 @@
       <c r="E42" s="14"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
       <formula1>AnalysisType</formula1>
     </dataValidation>
@@ -5795,9 +5834,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
       <formula1>Workflow</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B22">
-      <formula1>samplemethod</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17599,10 +17635,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A10"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17613,7 +17649,7 @@
     <col min="5" max="5" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>456</v>
       </c>
@@ -17624,7 +17660,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>446</v>
       </c>
@@ -17635,7 +17671,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>447</v>
       </c>
@@ -17646,7 +17682,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>454</v>
       </c>
@@ -17657,7 +17693,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>448</v>
       </c>
@@ -17668,7 +17704,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>661</v>
       </c>
@@ -17679,7 +17715,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>474</v>
       </c>
@@ -17690,7 +17726,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>472</v>
       </c>
@@ -17701,215 +17737,227 @@
         <v>602</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>637</v>
       </c>
       <c r="C12" t="s">
         <v>638</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>648</v>
       </c>
-      <c r="I12" t="s">
+      <c r="L12" t="s">
         <v>651</v>
       </c>
-      <c r="K12" t="s">
+      <c r="O12" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R12" s="37" t="s">
+        <v>641</v>
+      </c>
+      <c r="U12" s="37" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>638</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>662</v>
+      </c>
+      <c r="G13" t="s">
+        <v>474</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="J13" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="M13">
+        <v>30</v>
+      </c>
+      <c r="O13" t="s">
         <v>4</v>
       </c>
-      <c r="F13">
+      <c r="P13">
         <v>30</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="H13" s="36">
-        <v>0.01</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="J13">
-        <v>30</v>
-      </c>
-      <c r="K13" t="s">
-        <v>4</v>
-      </c>
-      <c r="L13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="H14" s="36">
+      <c r="J14" s="36">
         <v>0.01</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="L14" s="38" t="s">
         <v>656</v>
       </c>
-      <c r="J14">
+      <c r="M14">
         <v>5</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="O14" s="38" t="s">
         <v>656</v>
       </c>
-      <c r="L14">
+      <c r="P14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>600</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="H15" s="36">
+      <c r="J15" s="36">
         <v>45036000000000</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="J15">
+      <c r="M15">
         <v>3</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="O15" s="38" t="s">
         <v>657</v>
       </c>
-      <c r="L15">
+      <c r="P15">
         <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>640</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>100</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="J16" s="36">
+      <c r="M16" s="36">
         <v>0.01</v>
       </c>
-      <c r="K16" s="38" t="s">
+      <c r="O16" s="38" t="s">
         <v>658</v>
       </c>
-      <c r="L16">
+      <c r="P16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>639</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="J17" s="38" t="s">
         <v>598</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="J17" s="36">
+      <c r="M17" s="36">
         <v>0.01</v>
       </c>
-      <c r="K17" s="38" t="s">
+      <c r="O17" s="38" t="s">
         <v>659</v>
       </c>
-      <c r="L17">
+      <c r="P17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>641</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="H18" s="38">
-        <v>2</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="38">
+        <v>2</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="J18" s="36">
+      <c r="M18" s="36">
         <v>0.01</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="O18" s="38" t="s">
         <v>660</v>
       </c>
-      <c r="L18">
+      <c r="P18">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>642</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="J19" s="36">
+      <c r="M19" s="36">
         <v>45036000000000</v>
       </c>
-      <c r="K19" s="38" t="s">
+      <c r="O19" s="38" t="s">
         <v>597</v>
       </c>
-      <c r="L19" s="38" t="s">
+      <c r="P19" s="38" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I20" s="1" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L20" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="J20" s="37">
+      <c r="M20" s="37">
         <v>100</v>
       </c>
-      <c r="K20" s="38" t="s">
+      <c r="O20" s="38" t="s">
         <v>599</v>
       </c>
-      <c r="L20" s="38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I21" s="1" t="s">
+      <c r="P20" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L21" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="J21" s="38" t="s">
+      <c r="M21" s="38" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I22" s="1" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L22" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="J22" s="38">
+      <c r="M22" s="38">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating template for parsing directory name of measure
</commit_message>
<xml_diff>
--- a/doc/template_0_2_0.xlsx
+++ b/doc/template_0_2_0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-33540" yWindow="0" windowWidth="23256" windowHeight="5700" tabRatio="562" activeTab="5"/>
+    <workbookView xWindow="-33540" yWindow="0" windowWidth="23256" windowHeight="5700" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2539" uniqueCount="682">
   <si>
     <t>type</t>
   </si>
@@ -5423,7 +5423,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5938,9 +5938,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z96"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6025,7 +6025,9 @@
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="D3" s="11" t="s">
         <v>48</v>
       </c>
@@ -17715,7 +17717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated template for dir measure
</commit_message>
<xml_diff>
--- a/doc/template_0_2_0.xlsx
+++ b/doc/template_0_2_0.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2539" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2558" uniqueCount="682">
   <si>
     <t>type</t>
   </si>
@@ -5939,8 +5939,8 @@
   <dimension ref="A1:Z96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="3" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6135,7 +6135,9 @@
       <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="C6"/>
+      <c r="C6" s="37" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" t="s">
         <v>49</v>
       </c>
@@ -6436,7 +6438,9 @@
       <c r="B16" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="20" t="s">
+        <v>294</v>
+      </c>
       <c r="D16" s="20" t="s">
         <v>294</v>
       </c>
@@ -6746,6 +6750,9 @@
       <c r="B26" t="s">
         <v>75</v>
       </c>
+      <c r="C26" s="37" t="s">
+        <v>75</v>
+      </c>
       <c r="D26" t="s">
         <v>75</v>
       </c>
@@ -6886,7 +6893,9 @@
       <c r="B32" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="C32" s="20"/>
+      <c r="C32" s="20" t="s">
+        <v>196</v>
+      </c>
       <c r="D32" s="20" t="s">
         <v>196</v>
       </c>
@@ -7022,7 +7031,9 @@
       <c r="B36" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="C36" s="20"/>
+      <c r="C36" s="20" t="s">
+        <v>336</v>
+      </c>
       <c r="D36" s="20" t="s">
         <v>336</v>
       </c>
@@ -7112,7 +7123,9 @@
       <c r="B39" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="C39" s="20"/>
+      <c r="C39" s="20" t="s">
+        <v>225</v>
+      </c>
       <c r="D39" s="20" t="s">
         <v>225</v>
       </c>
@@ -7504,7 +7517,9 @@
       <c r="B54" s="20" t="s">
         <v>505</v>
       </c>
-      <c r="C54" s="20"/>
+      <c r="C54" s="20" t="s">
+        <v>394</v>
+      </c>
       <c r="D54" s="20" t="s">
         <v>394</v>
       </c>
@@ -7594,7 +7609,9 @@
       <c r="B57" s="20" t="s">
         <v>506</v>
       </c>
-      <c r="C57" s="20"/>
+      <c r="C57" s="20" t="s">
+        <v>394</v>
+      </c>
       <c r="D57" s="20" t="s">
         <v>394</v>
       </c>
@@ -7708,7 +7725,9 @@
       <c r="B60" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="C60" s="20"/>
+      <c r="C60" s="20" t="s">
+        <v>394</v>
+      </c>
       <c r="D60" s="20" t="s">
         <v>394</v>
       </c>
@@ -7822,7 +7841,9 @@
       <c r="B63" s="20" t="s">
         <v>508</v>
       </c>
-      <c r="C63" s="20"/>
+      <c r="C63" s="20" t="s">
+        <v>394</v>
+      </c>
       <c r="D63" s="20" t="s">
         <v>394</v>
       </c>
@@ -7936,7 +7957,9 @@
       <c r="B66" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="C66" s="20"/>
+      <c r="C66" s="20" t="s">
+        <v>394</v>
+      </c>
       <c r="D66" s="20" t="s">
         <v>394</v>
       </c>
@@ -8054,7 +8077,9 @@
       <c r="B69" t="s">
         <v>515</v>
       </c>
-      <c r="C69"/>
+      <c r="C69" s="37" t="s">
+        <v>516</v>
+      </c>
       <c r="D69" t="s">
         <v>516</v>
       </c>
@@ -8303,6 +8328,9 @@
       </c>
       <c r="B77" t="s">
         <v>263</v>
+      </c>
+      <c r="C77" s="37" t="s">
+        <v>264</v>
       </c>
       <c r="D77" t="s">
         <v>264</v>
@@ -8473,7 +8501,9 @@
       <c r="B83" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="C83" s="1"/>
+      <c r="C83" s="38" t="s">
+        <v>567</v>
+      </c>
       <c r="D83" s="1" t="s">
         <v>567</v>
       </c>
@@ -8571,6 +8601,9 @@
       <c r="B86" t="s">
         <v>578</v>
       </c>
+      <c r="C86" s="37" t="s">
+        <v>577</v>
+      </c>
       <c r="D86" t="s">
         <v>577</v>
       </c>
@@ -8659,6 +8692,9 @@
       <c r="B89" t="s">
         <v>584</v>
       </c>
+      <c r="C89" s="37" t="s">
+        <v>583</v>
+      </c>
       <c r="D89" t="s">
         <v>583</v>
       </c>
@@ -8710,6 +8746,9 @@
       <c r="B91" t="s">
         <v>590</v>
       </c>
+      <c r="C91" s="37" t="s">
+        <v>587</v>
+      </c>
       <c r="D91" t="s">
         <v>587</v>
       </c>
@@ -8761,6 +8800,9 @@
       <c r="B93" t="s">
         <v>576</v>
       </c>
+      <c r="C93" s="37" t="s">
+        <v>574</v>
+      </c>
       <c r="D93" t="s">
         <v>574</v>
       </c>
@@ -8812,7 +8854,9 @@
       <c r="B95" t="s">
         <v>561</v>
       </c>
-      <c r="C95"/>
+      <c r="C95" s="37" t="s">
+        <v>562</v>
+      </c>
       <c r="D95" t="s">
         <v>562</v>
       </c>

</xml_diff>

<commit_message>
updating formatatting to look better
</commit_message>
<xml_diff>
--- a/doc/template_0_2_0.xlsx
+++ b/doc/template_0_2_0.xlsx
@@ -5938,9 +5938,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5950,16 +5950,19 @@
     <col min="3" max="3" width="47" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.44140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" style="5" customWidth="1"/>
     <col min="11" max="11" width="7.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="7.77734375" style="1" customWidth="1"/>
-    <col min="16" max="19" width="11.44140625" style="1"/>
+    <col min="14" max="14" width="7.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="1" customWidth="1"/>
+    <col min="16" max="17" width="11.44140625" style="1"/>
+    <col min="18" max="18" width="13.5546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.44140625" style="1"/>
     <col min="20" max="20" width="46.109375" style="1" customWidth="1"/>
     <col min="21" max="23" width="11.44140625" style="1"/>
     <col min="24" max="24" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -5990,7 +5993,7 @@
         <v>502</v>
       </c>
       <c r="Q1" s="28"/>
-      <c r="R1" s="6"/>
+      <c r="R1" s="28"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="39" t="s">

</xml_diff>